<commit_message>
fix: repait wrong data
</commit_message>
<xml_diff>
--- a/docus/Assist TBD _ iZcy in TBD.xlsx
+++ b/docus/Assist TBD _ iZcy in TBD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions_All" sheetId="1" state="visible" r:id="rId2"/>
@@ -328,11 +328,11 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
@@ -1959,11 +1959,11 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
@@ -3589,11 +3589,11 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.75"/>
@@ -5219,11 +5219,11 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
@@ -5284,7 +5284,7 @@
         <v>1167</v>
       </c>
       <c r="H2" s="14" t="n">
-        <v>384</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5310,7 +5310,7 @@
         <v>1063</v>
       </c>
       <c r="H3" s="14" t="n">
-        <v>561</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5336,7 +5336,7 @@
         <v>1161</v>
       </c>
       <c r="H4" s="14" t="n">
-        <v>517</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5362,7 +5362,7 @@
         <v>1495</v>
       </c>
       <c r="H5" s="14" t="n">
-        <v>556</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5388,7 +5388,7 @@
         <v>1136</v>
       </c>
       <c r="H6" s="14" t="n">
-        <v>526</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5414,7 +5414,7 @@
         <v>1150</v>
       </c>
       <c r="H7" s="14" t="n">
-        <v>452</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5440,7 +5440,7 @@
         <v>1201</v>
       </c>
       <c r="H8" s="14" t="n">
-        <v>586</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5466,7 +5466,7 @@
         <v>1115</v>
       </c>
       <c r="H9" s="14" t="n">
-        <v>215</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5492,7 +5492,7 @@
         <v>1230</v>
       </c>
       <c r="H10" s="14" t="n">
-        <v>335</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5518,7 +5518,7 @@
         <v>1175</v>
       </c>
       <c r="H11" s="14" t="n">
-        <v>377</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5544,7 +5544,7 @@
         <v>1232</v>
       </c>
       <c r="H12" s="14" t="n">
-        <v>491</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5570,7 +5570,7 @@
         <v>1201</v>
       </c>
       <c r="H13" s="14" t="n">
-        <v>462</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5596,7 +5596,7 @@
         <v>1294</v>
       </c>
       <c r="H14" s="14" t="n">
-        <v>475</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5622,7 +5622,7 @@
         <v>1117</v>
       </c>
       <c r="H15" s="14" t="n">
-        <v>421</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5648,7 +5648,7 @@
         <v>1215</v>
       </c>
       <c r="H16" s="14" t="n">
-        <v>341</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5674,7 +5674,7 @@
         <v>1290</v>
       </c>
       <c r="H17" s="14" t="n">
-        <v>174</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5700,7 +5700,7 @@
         <v>1111</v>
       </c>
       <c r="H18" s="14" t="n">
-        <v>513</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5726,7 +5726,7 @@
         <v>1180</v>
       </c>
       <c r="H19" s="14" t="n">
-        <v>370</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5752,7 +5752,7 @@
         <v>1144</v>
       </c>
       <c r="H20" s="14" t="n">
-        <v>518</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5778,7 +5778,7 @@
         <v>1100</v>
       </c>
       <c r="H21" s="14" t="n">
-        <v>295</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5804,7 +5804,7 @@
         <v>1317</v>
       </c>
       <c r="H22" s="14" t="n">
-        <v>486</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5830,7 +5830,7 @@
         <v>1314</v>
       </c>
       <c r="H23" s="14" t="n">
-        <v>398</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5856,7 +5856,7 @@
         <v>1332</v>
       </c>
       <c r="H24" s="14" t="n">
-        <v>361</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5882,7 +5882,7 @@
         <v>1132</v>
       </c>
       <c r="H25" s="14" t="n">
-        <v>523</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5908,7 +5908,7 @@
         <v>1156</v>
       </c>
       <c r="H26" s="14" t="n">
-        <v>409</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5934,7 +5934,7 @@
         <v>1141</v>
       </c>
       <c r="H27" s="14" t="n">
-        <v>530</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5960,7 +5960,7 @@
         <v>1344</v>
       </c>
       <c r="H28" s="14" t="n">
-        <v>371</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5986,7 +5986,7 @@
         <v>1126</v>
       </c>
       <c r="H29" s="14" t="n">
-        <v>548</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6012,7 +6012,7 @@
         <v>1315</v>
       </c>
       <c r="H30" s="14" t="n">
-        <v>516</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6038,7 +6038,7 @@
         <v>1214</v>
       </c>
       <c r="H31" s="14" t="n">
-        <v>477</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6064,7 +6064,7 @@
         <v>1350</v>
       </c>
       <c r="H32" s="14" t="n">
-        <v>666</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6090,7 +6090,7 @@
         <v>1142</v>
       </c>
       <c r="H33" s="14" t="n">
-        <v>601</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6116,7 +6116,7 @@
         <v>1127</v>
       </c>
       <c r="H34" s="14" t="n">
-        <v>416</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6142,7 +6142,7 @@
         <v>1178</v>
       </c>
       <c r="H35" s="14" t="n">
-        <v>418</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6168,7 +6168,7 @@
         <v>1155</v>
       </c>
       <c r="H36" s="14" t="n">
-        <v>583</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6194,7 +6194,7 @@
         <v>1254</v>
       </c>
       <c r="H37" s="14" t="n">
-        <v>356</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6220,7 +6220,7 @@
         <v>1201</v>
       </c>
       <c r="H38" s="14" t="n">
-        <v>490</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6246,7 +6246,7 @@
         <v>1291</v>
       </c>
       <c r="H39" s="14" t="n">
-        <v>494</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6272,7 +6272,7 @@
         <v>1287</v>
       </c>
       <c r="H40" s="14" t="n">
-        <v>559</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6298,7 +6298,7 @@
         <v>1151</v>
       </c>
       <c r="H41" s="14" t="n">
-        <v>543</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6324,7 +6324,7 @@
         <v>1144</v>
       </c>
       <c r="H42" s="14" t="n">
-        <v>188</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6350,7 +6350,7 @@
         <v>1116</v>
       </c>
       <c r="H43" s="14" t="n">
-        <v>539</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6376,7 +6376,7 @@
         <v>1122</v>
       </c>
       <c r="H44" s="14" t="n">
-        <v>396</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6402,7 +6402,7 @@
         <v>1294</v>
       </c>
       <c r="H45" s="14" t="n">
-        <v>470</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6428,7 +6428,7 @@
         <v>1279</v>
       </c>
       <c r="H46" s="14" t="n">
-        <v>307</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6454,7 +6454,7 @@
         <v>1210</v>
       </c>
       <c r="H47" s="14" t="n">
-        <v>473</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6480,7 +6480,7 @@
         <v>1116</v>
       </c>
       <c r="H48" s="14" t="n">
-        <v>291</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6506,7 +6506,7 @@
         <v>1158</v>
       </c>
       <c r="H49" s="14" t="n">
-        <v>336</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6532,7 +6532,7 @@
         <v>1116</v>
       </c>
       <c r="H50" s="14" t="n">
-        <v>171</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6558,7 +6558,7 @@
         <v>1208</v>
       </c>
       <c r="H51" s="14" t="n">
-        <v>473</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6584,7 +6584,7 @@
         <v>1180</v>
       </c>
       <c r="H52" s="14" t="n">
-        <v>540</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6610,7 +6610,7 @@
         <v>1123</v>
       </c>
       <c r="H53" s="14" t="n">
-        <v>439</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6636,7 +6636,7 @@
         <v>1281</v>
       </c>
       <c r="H54" s="14" t="n">
-        <v>399</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6662,7 +6662,7 @@
         <v>1250</v>
       </c>
       <c r="H55" s="14" t="n">
-        <v>603</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6688,7 +6688,7 @@
         <v>1210</v>
       </c>
       <c r="H56" s="14" t="n">
-        <v>280</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6714,7 +6714,7 @@
         <v>1140</v>
       </c>
       <c r="H57" s="14" t="n">
-        <v>550</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6740,7 +6740,7 @@
         <v>1113</v>
       </c>
       <c r="H58" s="14" t="n">
-        <v>428</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6766,7 +6766,7 @@
         <v>1159</v>
       </c>
       <c r="H59" s="14" t="n">
-        <v>369</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6792,7 +6792,7 @@
         <v>1146</v>
       </c>
       <c r="H60" s="14" t="n">
-        <v>506</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6818,7 +6818,7 @@
         <v>1175</v>
       </c>
       <c r="H61" s="17" t="n">
-        <v>523</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6849,11 +6849,11 @@
   </sheetPr>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.38"/>
@@ -8109,8 +8109,8 @@
   </sheetPr>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>